<commit_message>
Minor typos, but great new plots
Here are the cross Cond (not laryngeal Pos) This just averages across all of a AudFb type
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/LarynxPos/LarynxPosStat.xlsx
+++ b/Results/Pooled Analyses/LarynxPos/LarynxPosStat.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsmith\Documents\MATLAB\Dissociating-Role-of-Feedback-in-Voice-Motor-Control\Results\Pooled Analyses\LarynxPos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,7 +323,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>